<commit_message>
Mark on ClueLayout. Add targets tests as required.
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsh/eclipse-projects/ClueGames/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A771C4DE-1893-F84E-97F8-B4538581F80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{88296155-C220-3E49-BEF8-0D37CED2594E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="961" uniqueCount="37">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="968" uniqueCount="44">
   <si>
     <t>AE</t>
   </si>
@@ -136,6 +136,27 @@
   </si>
   <si>
     <t>EA</t>
+  </si>
+  <si>
+    <t>Number of doors: 32</t>
+  </si>
+  <si>
+    <t>White: door direction tests (FileInitTest)</t>
+  </si>
+  <si>
+    <t>Light grey: room tests (FileInitTest)</t>
+  </si>
+  <si>
+    <t>Light orange: adjacency from room and doors</t>
+  </si>
+  <si>
+    <t>Dark orange: adjacency walkways</t>
+  </si>
+  <si>
+    <t>Light blue: test targets</t>
+  </si>
+  <si>
+    <t>Red: test targets occupied</t>
   </si>
 </sst>
 </file>
@@ -278,7 +299,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,6 +512,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,7 +706,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -663,6 +714,12 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1018,15 +1075,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE31"/>
+  <dimension ref="A1:AG31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AK8" sqref="AK8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.6640625" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="33" max="33" width="41.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +1123,7 @@
       <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -1120,8 +1180,11 @@
       <c r="AE1" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="AG1" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1167,7 +1230,7 @@
       <c r="O2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q2" s="1" t="s">
@@ -1215,8 +1278,11 @@
       <c r="AE2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="AG2" s="8" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1244,7 +1310,7 @@
       <c r="I3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -1298,7 +1364,7 @@
       <c r="AA3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AB3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="AC3" s="2" t="s">
@@ -1310,8 +1376,11 @@
       <c r="AE3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="AG3" s="10" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1321,7 +1390,7 @@
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1393,7 +1462,7 @@
       <c r="AA4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB4" s="4" t="s">
+      <c r="AB4" s="12" t="s">
         <v>10</v>
       </c>
       <c r="AC4" s="2" t="s">
@@ -1406,7 +1475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1500,12 +1569,15 @@
       <c r="AE5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="AG5" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1523,7 +1595,7 @@
       <c r="G6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -1571,7 +1643,7 @@
       <c r="W6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X6" s="6" t="s">
+      <c r="X6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="Y6" s="2" t="s">
@@ -1595,8 +1667,11 @@
       <c r="AE6" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="AG6" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="7" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1627,7 +1702,7 @@
       <c r="J7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -1642,7 +1717,7 @@
       <c r="O7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="10" t="s">
         <v>15</v>
       </c>
       <c r="Q7" s="2" t="s">
@@ -1657,7 +1732,7 @@
       <c r="T7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="U7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="V7" s="3" t="s">
@@ -1690,8 +1765,11 @@
       <c r="AE7" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="AG7" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="8" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1707,7 +1785,7 @@
       <c r="E8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1767,7 +1845,7 @@
       <c r="Y8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Z8" s="6" t="s">
+      <c r="Z8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="AA8" s="1" t="s">
@@ -1785,8 +1863,11 @@
       <c r="AE8" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="AG8" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="9" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1805,19 +1886,19 @@
       <c r="F9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="10" t="s">
         <v>2</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="7" t="s">
         <v>2</v>
       </c>
       <c r="L9" s="2" t="s">
@@ -1881,7 +1962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1909,13 +1990,13 @@
       <c r="I10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="1" t="s">
+      <c r="K10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="12" t="s">
         <v>2</v>
       </c>
       <c r="M10" s="2" t="s">
@@ -1976,7 +2057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1995,7 +2076,7 @@
       <c r="F11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -2049,7 +2130,7 @@
       <c r="X11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Y11" s="6" t="s">
+      <c r="Y11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Z11" s="1" t="s">
@@ -2071,7 +2152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2114,13 +2195,13 @@
       <c r="N12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q12" s="6" t="s">
+      <c r="Q12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="R12" s="1" t="s">
@@ -2135,7 +2216,7 @@
       <c r="U12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="V12" s="12" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="2" t="s">
@@ -2166,7 +2247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2206,7 +2287,7 @@
       <c r="M13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N13" s="6" t="s">
+      <c r="N13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="O13" s="2" t="s">
@@ -2218,7 +2299,7 @@
       <c r="Q13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R13" s="6" t="s">
+      <c r="R13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="S13" s="1" t="s">
@@ -2261,7 +2342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -2316,10 +2397,10 @@
       <c r="R14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S14" s="6" t="s">
+      <c r="S14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="T14" s="12" t="s">
         <v>2</v>
       </c>
       <c r="U14" s="2" t="s">
@@ -2356,7 +2437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -2390,7 +2471,7 @@
       <c r="K15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="M15" s="2" t="s">
@@ -2414,7 +2495,7 @@
       <c r="S15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T15" s="6" t="s">
+      <c r="T15" s="7" t="s">
         <v>14</v>
       </c>
       <c r="U15" s="2" t="s">
@@ -2451,11 +2532,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -2503,7 +2584,7 @@
       <c r="Q16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R16" s="2" t="s">
+      <c r="R16" s="11" t="s">
         <v>19</v>
       </c>
       <c r="S16" s="2" t="s">
@@ -2524,7 +2605,7 @@
       <c r="X16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Y16" s="4" t="s">
+      <c r="Y16" s="12" t="s">
         <v>25</v>
       </c>
       <c r="Z16" s="2" t="s">
@@ -2539,7 +2620,7 @@
       <c r="AC16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD16" s="6" t="s">
+      <c r="AD16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="AE16" s="1" t="s">
@@ -2580,7 +2661,7 @@
       <c r="K17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="L17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -2604,7 +2685,7 @@
       <c r="S17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T17" s="6" t="s">
+      <c r="T17" s="7" t="s">
         <v>14</v>
       </c>
       <c r="U17" s="2" t="s">
@@ -2678,7 +2759,7 @@
       <c r="L18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="M18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="N18" s="2" t="s">
@@ -2770,7 +2851,7 @@
       <c r="K19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L19" s="12" t="s">
         <v>2</v>
       </c>
       <c r="M19" s="1" t="s">
@@ -2788,7 +2869,7 @@
       <c r="Q19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R19" s="6" t="s">
+      <c r="R19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="S19" s="1" t="s">
@@ -2841,7 +2922,7 @@
       <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="7" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -2874,13 +2955,13 @@
       <c r="N20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O20" s="6" t="s">
+      <c r="O20" s="11" t="s">
         <v>5</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q20" s="6" t="s">
+      <c r="Q20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="R20" s="1" t="s">
@@ -2939,13 +3020,13 @@
       <c r="D21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="12" t="s">
         <v>2</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="7" t="s">
         <v>16</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -2984,7 +3065,7 @@
       <c r="S21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T21" s="1" t="s">
+      <c r="T21" s="12" t="s">
         <v>2</v>
       </c>
       <c r="U21" s="3" t="s">
@@ -2999,7 +3080,7 @@
       <c r="X21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Y21" s="6" t="s">
+      <c r="Y21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="Z21" s="1" t="s">
@@ -3112,7 +3193,7 @@
       <c r="AD22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AE22" s="1" t="s">
+      <c r="AE22" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -3227,7 +3308,7 @@
       <c r="E24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="11" t="s">
         <v>5</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -3287,7 +3368,7 @@
       <c r="Y24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Z24" s="6" t="s">
+      <c r="Z24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="AA24" s="1" t="s">
@@ -3337,7 +3418,7 @@
       <c r="J25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K25" s="6" t="s">
+      <c r="K25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L25" s="2" t="s">
@@ -3352,7 +3433,7 @@
       <c r="O25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P25" s="4" t="s">
+      <c r="P25" s="12" t="s">
         <v>30</v>
       </c>
       <c r="Q25" s="2" t="s">
@@ -3367,7 +3448,7 @@
       <c r="T25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="U25" s="6" t="s">
+      <c r="U25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="V25" s="3" t="s">
@@ -3423,7 +3504,7 @@
       <c r="G26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -3471,7 +3552,7 @@
       <c r="W26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X26" s="6" t="s">
+      <c r="X26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="Y26" s="2" t="s">
@@ -3827,7 +3908,7 @@
       <c r="O30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P30" s="6" t="s">
+      <c r="P30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="Q30" s="1" t="s">
@@ -3877,7 +3958,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -3952,7 +4033,7 @@
       <c r="Y31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Z31" s="2" t="s">
+      <c r="Z31" s="11" t="s">
         <v>28</v>
       </c>
       <c r="AA31" s="2" t="s">
@@ -3967,7 +4048,7 @@
       <c r="AD31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE31" s="5" t="s">
+      <c r="AE31" s="10" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add nested recursive calTarget method in Board class. Add occupied status getter in BoardCell class. Correct some expected result of some test in BoardAdjTargetTest.
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsh/eclipse-projects/ClueGames/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{88296155-C220-3E49-BEF8-0D37CED2594E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DEBE4565-A373-AA40-B0A0-840D787577B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -299,7 +299,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -542,6 +542,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -716,10 +722,10 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1078,7 +1084,7 @@
   <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.6640625" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1180,7 +1186,7 @@
       <c r="AE1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AG1" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1364,7 +1370,7 @@
       <c r="AA3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="AB3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="AC3" s="2" t="s">
@@ -1376,7 +1382,7 @@
       <c r="AE3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AG3" s="10" t="s">
+      <c r="AG3" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1390,7 +1396,7 @@
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -1462,7 +1468,7 @@
       <c r="AA4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AB4" s="12" t="s">
+      <c r="AB4" s="11" t="s">
         <v>10</v>
       </c>
       <c r="AC4" s="2" t="s">
@@ -1569,7 +1575,7 @@
       <c r="AE5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AG5" s="11" t="s">
+      <c r="AG5" s="10" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1577,7 +1583,7 @@
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1717,7 +1723,7 @@
       <c r="O7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="P7" s="9" t="s">
         <v>15</v>
       </c>
       <c r="Q7" s="2" t="s">
@@ -1765,7 +1771,7 @@
       <c r="AE7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AG7" s="12" t="s">
+      <c r="AG7" s="11" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1886,13 +1892,13 @@
       <c r="F9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="9" t="s">
         <v>2</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -1990,13 +1996,13 @@
       <c r="I10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="12" t="s">
+      <c r="K10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" s="11" t="s">
         <v>2</v>
       </c>
       <c r="M10" s="2" t="s">
@@ -2216,7 +2222,7 @@
       <c r="U12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="V12" s="12" t="s">
+      <c r="V12" s="11" t="s">
         <v>2</v>
       </c>
       <c r="W12" s="2" t="s">
@@ -2400,7 +2406,7 @@
       <c r="S14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T14" s="12" t="s">
+      <c r="T14" s="11" t="s">
         <v>2</v>
       </c>
       <c r="U14" s="2" t="s">
@@ -2584,7 +2590,7 @@
       <c r="Q16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="R16" s="10" t="s">
         <v>19</v>
       </c>
       <c r="S16" s="2" t="s">
@@ -2605,7 +2611,7 @@
       <c r="X16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Y16" s="12" t="s">
+      <c r="Y16" s="11" t="s">
         <v>25</v>
       </c>
       <c r="Z16" s="2" t="s">
@@ -2851,7 +2857,7 @@
       <c r="K19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L19" s="12" t="s">
+      <c r="L19" s="11" t="s">
         <v>2</v>
       </c>
       <c r="M19" s="1" t="s">
@@ -2955,7 +2961,7 @@
       <c r="N20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O20" s="11" t="s">
+      <c r="O20" s="10" t="s">
         <v>5</v>
       </c>
       <c r="P20" s="1" t="s">
@@ -3020,7 +3026,7 @@
       <c r="D21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -3065,7 +3071,7 @@
       <c r="S21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T21" s="12" t="s">
+      <c r="T21" s="11" t="s">
         <v>2</v>
       </c>
       <c r="U21" s="3" t="s">
@@ -3308,7 +3314,7 @@
       <c r="E24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>5</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -3433,7 +3439,7 @@
       <c r="O25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P25" s="12" t="s">
+      <c r="P25" s="11" t="s">
         <v>30</v>
       </c>
       <c r="Q25" s="2" t="s">
@@ -3958,7 +3964,7 @@
       </c>
     </row>
     <row r="31" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -4033,7 +4039,7 @@
       <c r="Y31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Z31" s="11" t="s">
+      <c r="Z31" s="10" t="s">
         <v>28</v>
       </c>
       <c r="AA31" s="2" t="s">
@@ -4048,7 +4054,7 @@
       <c r="AD31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE31" s="10" t="s">
+      <c r="AE31" s="9" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ClueGame.java which prints the board's map. Map currently has walkways, rooms, unwalkable cells, and doors implimented. -Michael
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsh/eclipse-projects/ClueGames/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Eclips\Clue\ClueMain\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DEBE4565-A373-AA40-B0A0-840D787577B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E0FCE6FA-3BA3-40A3-AA29-9419E6489EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClueLayout" sheetId="1" r:id="rId1"/>
@@ -1084,15 +1084,15 @@
   <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.6640625" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="33" max="33" width="41.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2952,8 +2952,8 @@
       <c r="K20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>2</v>
+      <c r="L20" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>2</v>
@@ -3013,7 +3013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Computer and human player suggestions compleated, and human accusations compleated. -M
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Eclips\Clue\ClueMain\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E0FCE6FA-3BA3-40A3-AA29-9419E6489EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BAF21DB3-6A45-403C-8435-718653E53CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ClueLayout" sheetId="1" r:id="rId1"/>
@@ -1084,7 +1084,7 @@
   <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.6640625" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1705,8 +1705,8 @@
       <c r="I7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>11</v>
+      <c r="J7" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>14</v>
@@ -1741,8 +1741,8 @@
       <c r="U7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V7" s="3" t="s">
-        <v>11</v>
+      <c r="V7" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>2</v>
@@ -1987,8 +1987,8 @@
       <c r="F10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>11</v>
+      <c r="G10" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>2</v>
@@ -2041,8 +2041,8 @@
       <c r="X10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Y10" s="3" t="s">
-        <v>11</v>
+      <c r="Y10" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="Z10" s="3" t="s">
         <v>11</v>
@@ -3127,8 +3127,8 @@
       <c r="F22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>11</v>
+      <c r="G22" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>2</v>
@@ -3181,8 +3181,8 @@
       <c r="X22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Y22" s="3" t="s">
-        <v>11</v>
+      <c r="Y22" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="Z22" s="3" t="s">
         <v>11</v>
@@ -3421,8 +3421,8 @@
       <c r="I25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J25" s="3" t="s">
-        <v>11</v>
+      <c r="J25" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>14</v>
@@ -3457,8 +3457,8 @@
       <c r="U25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V25" s="3" t="s">
-        <v>11</v>
+      <c r="V25" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="W25" s="1" t="s">
         <v>2</v>

</xml_diff>